<commit_message>
Incomplete, but does not error out
</commit_message>
<xml_diff>
--- a/Color System.xlsx
+++ b/Color System.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mika/Documents/Side Projects for self/circus-organizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D56AAD-EEB9-B042-90E4-9CE7DED528E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13169ED-A770-A342-BC7B-8F9FA41FED22}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16480" xr2:uid="{1DAADBF5-1F96-DA4F-8DD1-B98C6FAFC088}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="13440" windowHeight="16460" xr2:uid="{1DAADBF5-1F96-DA4F-8DD1-B98C6FAFC088}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -518,7 +518,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>